<commit_message>
Add summary tag with label in group feature
</commit_message>
<xml_diff>
--- a/tests/Templates/GroupTagTests_FormulasWithTagsInGroupRow.xlsx
+++ b/tests/Templates/GroupTagTests_FormulasWithTagsInGroupRow.xlsx
@@ -79,10 +79,10 @@
     <t>Company</t>
   </si>
   <si>
-    <t>&lt;&lt;sum&gt;&gt;</t>
-  </si>
-  <si>
     <t>&lt;&lt;group TotalLabel="" GrandLabel=""&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&amp;="Total: "&lt;&lt;sum&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -900,7 +900,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="16" t="s">
@@ -909,7 +909,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="10"/>
       <c r="G6" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="15"/>

</xml_diff>